<commit_message>
Modified some portion of the code
</commit_message>
<xml_diff>
--- a/teacher_utility/Attendance_and_marks_ipl[B1].xlsx
+++ b/teacher_utility/Attendance_and_marks_ipl[B1].xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Codes\Python_Small_Projects\teacher_utility\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73FE6BEA-30C3-4FAA-8332-0B9E52988254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -28,251 +22,251 @@
     <t>Student Name</t>
   </si>
   <si>
-    <t>24-59065-3</t>
-  </si>
-  <si>
-    <t>25-60525-1</t>
-  </si>
-  <si>
-    <t>25-60526-1</t>
-  </si>
-  <si>
-    <t>25-60528-1</t>
-  </si>
-  <si>
-    <t>25-60530-1</t>
-  </si>
-  <si>
-    <t>25-60532-1</t>
-  </si>
-  <si>
-    <t>25-60534-1</t>
-  </si>
-  <si>
-    <t>25-60541-1</t>
-  </si>
-  <si>
-    <t>25-60542-1</t>
-  </si>
-  <si>
-    <t>25-60547-1</t>
-  </si>
-  <si>
-    <t>25-60548-1</t>
-  </si>
-  <si>
-    <t>25-60555-1</t>
-  </si>
-  <si>
-    <t>25-60559-1</t>
-  </si>
-  <si>
-    <t>25-60562-1</t>
-  </si>
-  <si>
-    <t>25-60565-1</t>
-  </si>
-  <si>
-    <t>25-60567-1</t>
-  </si>
-  <si>
-    <t>25-60568-1</t>
-  </si>
-  <si>
-    <t>25-60569-1</t>
-  </si>
-  <si>
-    <t>25-60571-1</t>
-  </si>
-  <si>
-    <t>25-60572-1</t>
-  </si>
-  <si>
-    <t>25-60575-1</t>
-  </si>
-  <si>
-    <t>25-60576-1</t>
-  </si>
-  <si>
-    <t>25-60579-1</t>
-  </si>
-  <si>
-    <t>25-60580-1</t>
-  </si>
-  <si>
-    <t>25-60583-1</t>
-  </si>
-  <si>
-    <t>25-60584-1</t>
-  </si>
-  <si>
-    <t>25-60587-1</t>
-  </si>
-  <si>
-    <t>25-60590-1</t>
-  </si>
-  <si>
-    <t>25-60591-1</t>
-  </si>
-  <si>
-    <t>25-60592-1</t>
-  </si>
-  <si>
-    <t>25-60593-1</t>
-  </si>
-  <si>
-    <t>25-60594-1</t>
-  </si>
-  <si>
-    <t>25-60601-1</t>
-  </si>
-  <si>
-    <t>25-60605-1</t>
-  </si>
-  <si>
-    <t>25-60607-1</t>
-  </si>
-  <si>
-    <t>25-60608-1</t>
-  </si>
-  <si>
-    <t>25-60610-1</t>
-  </si>
-  <si>
-    <t>25-60632-1</t>
-  </si>
-  <si>
-    <t>25-60633-1</t>
-  </si>
-  <si>
-    <t>25-60634-1</t>
-  </si>
-  <si>
-    <t>AZAD, NAHID AL</t>
-  </si>
-  <si>
-    <t>NAHREEN, WADIFA</t>
-  </si>
-  <si>
-    <t>SARA, JANNATUL MAWA</t>
-  </si>
-  <si>
-    <t>MAHADI, SAMIT HOSSAIN</t>
-  </si>
-  <si>
-    <t>CHISIM, MARK AMIO</t>
-  </si>
-  <si>
-    <t>OINDRILA, ANTORA TASNIM</t>
-  </si>
-  <si>
-    <t>KHAN, JAMIL AHMED</t>
-  </si>
-  <si>
-    <t>FUAD, MD.IKHTEAR UDDIN</t>
-  </si>
-  <si>
-    <t>MIM, SABEKUN NAHAR</t>
-  </si>
-  <si>
-    <t>JAHANGIR, RIFAT</t>
-  </si>
-  <si>
-    <t>ISLAM, TALHA</t>
-  </si>
-  <si>
-    <t>RUPA, AFROJA AKTER</t>
-  </si>
-  <si>
-    <t>MOLLAH, MD. MAHMUDUL HASAN SAJID</t>
-  </si>
-  <si>
-    <t>ZUBAYER, MD. HASNAIN AL</t>
-  </si>
-  <si>
-    <t>ISLAM, RASIDUL</t>
-  </si>
-  <si>
-    <t>TAMIM, RUMMAN TAHSIN</t>
-  </si>
-  <si>
-    <t>AHMED, RIDWAN</t>
-  </si>
-  <si>
-    <t>HASAN, MD. MAHADI</t>
-  </si>
-  <si>
-    <t>TALUKDER, MAISHA LAMYEA</t>
-  </si>
-  <si>
-    <t>RIFA, TANAYA AHMED</t>
-  </si>
-  <si>
-    <t>MALIHA, MAYSHA</t>
-  </si>
-  <si>
-    <t>NIHAL, MD. NAFISH HASAN</t>
-  </si>
-  <si>
-    <t>SARKER, DIPU KANTI</t>
-  </si>
-  <si>
-    <t>TITLY, ADILAH RAHMAN</t>
-  </si>
-  <si>
-    <t>SAHA, TANUSHREE</t>
-  </si>
-  <si>
-    <t>HASAN, ADIBA</t>
-  </si>
-  <si>
-    <t>SULTANA, SAIMA</t>
-  </si>
-  <si>
-    <t>RAHMAN, MD.TOHIDUR</t>
-  </si>
-  <si>
-    <t>HAQUE, FARHAN HASEEN</t>
-  </si>
-  <si>
-    <t>MUSTAKIM, MOHAMMAD</t>
-  </si>
-  <si>
-    <t>SAMADDER, SHIMUL</t>
-  </si>
-  <si>
-    <t>SHEFA, SANJIDA RABAB</t>
-  </si>
-  <si>
-    <t>RAD, RAFSAN JAHIN</t>
-  </si>
-  <si>
-    <t>RAFI, MD. IMAM HOSSAIN</t>
-  </si>
-  <si>
-    <t>KABIR, NUWAISIR</t>
-  </si>
-  <si>
-    <t>SHAISHAB, AYEAD BIN ALAM</t>
-  </si>
-  <si>
-    <t>MOHONA, MALIHA TASNIM</t>
-  </si>
-  <si>
-    <t>FARHAN, SHEKH</t>
-  </si>
-  <si>
-    <t>DAS, APON KRISHNA</t>
-  </si>
-  <si>
-    <t>SIDDIQUI, A.M. SAYEM</t>
+    <t>25-61411-1</t>
+  </si>
+  <si>
+    <t>25-61413-1</t>
+  </si>
+  <si>
+    <t>25-61414-1</t>
+  </si>
+  <si>
+    <t>25-61416-1</t>
+  </si>
+  <si>
+    <t>25-61417-1</t>
+  </si>
+  <si>
+    <t>25-61419-1</t>
+  </si>
+  <si>
+    <t>25-61420-1</t>
+  </si>
+  <si>
+    <t>25-61421-1</t>
+  </si>
+  <si>
+    <t>25-61425-1</t>
+  </si>
+  <si>
+    <t>25-61426-1</t>
+  </si>
+  <si>
+    <t>25-61428-1</t>
+  </si>
+  <si>
+    <t>25-61432-1</t>
+  </si>
+  <si>
+    <t>25-61433-1</t>
+  </si>
+  <si>
+    <t>25-61435-1</t>
+  </si>
+  <si>
+    <t>25-61439-1</t>
+  </si>
+  <si>
+    <t>25-61440-1</t>
+  </si>
+  <si>
+    <t>25-61441-1</t>
+  </si>
+  <si>
+    <t>25-61443-1</t>
+  </si>
+  <si>
+    <t>25-61445-1</t>
+  </si>
+  <si>
+    <t>25-61446-1</t>
+  </si>
+  <si>
+    <t>25-61455-1</t>
+  </si>
+  <si>
+    <t>25-61464-1</t>
+  </si>
+  <si>
+    <t>25-61467-1</t>
+  </si>
+  <si>
+    <t>25-61469-1</t>
+  </si>
+  <si>
+    <t>25-61470-1</t>
+  </si>
+  <si>
+    <t>25-61474-1</t>
+  </si>
+  <si>
+    <t>25-61480-1</t>
+  </si>
+  <si>
+    <t>25-61482-1</t>
+  </si>
+  <si>
+    <t>25-61483-1</t>
+  </si>
+  <si>
+    <t>25-61486-1</t>
+  </si>
+  <si>
+    <t>25-61488-1</t>
+  </si>
+  <si>
+    <t>25-61489-1</t>
+  </si>
+  <si>
+    <t>25-61490-1</t>
+  </si>
+  <si>
+    <t>25-61492-1</t>
+  </si>
+  <si>
+    <t>25-61495-1</t>
+  </si>
+  <si>
+    <t>25-61497-1</t>
+  </si>
+  <si>
+    <t>25-61499-1</t>
+  </si>
+  <si>
+    <t>25-61500-1</t>
+  </si>
+  <si>
+    <t>25-61501-1</t>
+  </si>
+  <si>
+    <t>25-61502-1</t>
+  </si>
+  <si>
+    <t>ROY, NILOY</t>
+  </si>
+  <si>
+    <t>MUNNA, MD. MAHARABUL ISLAM</t>
+  </si>
+  <si>
+    <t>TAUSI, SAMIA ISLAM</t>
+  </si>
+  <si>
+    <t>JUBAER, ABDULLAH</t>
+  </si>
+  <si>
+    <t>MITHILA, MYMUNA RAHMAN</t>
+  </si>
+  <si>
+    <t>ROY, POPY</t>
+  </si>
+  <si>
+    <t>ROMEL, RIDUONE KOWSAR</t>
+  </si>
+  <si>
+    <t>SABAH, SAMIN</t>
+  </si>
+  <si>
+    <t>AHMED, SAKIB</t>
+  </si>
+  <si>
+    <t>PAUL, AMI</t>
+  </si>
+  <si>
+    <t>SAKI, SABIKUN NAHAR</t>
+  </si>
+  <si>
+    <t>BARSHAN, SHARAR MOSTAFA</t>
+  </si>
+  <si>
+    <t>AHMED, KAZI SAJID</t>
+  </si>
+  <si>
+    <t>HASAN, RAKIBUL</t>
+  </si>
+  <si>
+    <t>THUN, AUNG LEIN</t>
+  </si>
+  <si>
+    <t>ANAN, NISHAT</t>
+  </si>
+  <si>
+    <t>ALIF, KANIZ MARZIA</t>
+  </si>
+  <si>
+    <t>DAS, ANOL</t>
+  </si>
+  <si>
+    <t>SARKER, SHARMIN HAQUE</t>
+  </si>
+  <si>
+    <t>RIDETA, SANJIDA RAHAMAN</t>
+  </si>
+  <si>
+    <t>KHAN, MD SAMIR</t>
+  </si>
+  <si>
+    <t>MRIDHA, MOHEB BILLAH</t>
+  </si>
+  <si>
+    <t>SHAHRIAR, TAHMID</t>
+  </si>
+  <si>
+    <t>ADOR, MD RADWAN AHAMMED</t>
+  </si>
+  <si>
+    <t>ISLAM, SAMANTHA</t>
+  </si>
+  <si>
+    <t>NIBIR, MIR MD FAKHRUL AZAM</t>
+  </si>
+  <si>
+    <t>AYSHE, TAMANNA BARI</t>
+  </si>
+  <si>
+    <t>MAHIN, MAKSUD</t>
+  </si>
+  <si>
+    <t>ORNOB, JIHADUL MOTIN</t>
+  </si>
+  <si>
+    <t>MAHI, IMTIYAZ MAHMUD</t>
+  </si>
+  <si>
+    <t>BHUIYAN, NASBIRUL ISLAM</t>
+  </si>
+  <si>
+    <t>RAFI, MD ABDULLAH AL</t>
+  </si>
+  <si>
+    <t>OMAR, MD. SABID</t>
+  </si>
+  <si>
+    <t>NOMAN, FARDIN</t>
+  </si>
+  <si>
+    <t>RIJOY, MD. MOINUL HOSSAIN</t>
+  </si>
+  <si>
+    <t>MAJUMDER, SUJOY</t>
+  </si>
+  <si>
+    <t>ONI, MD RADOAN AHMED</t>
+  </si>
+  <si>
+    <t>MUKTA, HIRA MONI</t>
+  </si>
+  <si>
+    <t>SHAHRIYAR, MD MOSTAK</t>
+  </si>
+  <si>
+    <t>KARMAKER, SONDIPON</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,12 +278,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -341,14 +329,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -395,7 +375,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,27 +407,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -479,24 +441,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -672,20 +616,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -693,7 +631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -701,7 +639,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -709,7 +647,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -717,7 +655,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -725,7 +663,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -733,7 +671,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -741,7 +679,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3">
       <c r="B10" t="s">
         <v>8</v>
       </c>
@@ -749,7 +687,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3">
       <c r="B11" t="s">
         <v>9</v>
       </c>
@@ -757,7 +695,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3">
       <c r="B12" t="s">
         <v>10</v>
       </c>
@@ -765,7 +703,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3">
       <c r="B13" t="s">
         <v>11</v>
       </c>
@@ -773,7 +711,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3">
       <c r="B14" t="s">
         <v>12</v>
       </c>
@@ -781,7 +719,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3">
       <c r="B15" t="s">
         <v>13</v>
       </c>
@@ -789,7 +727,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3">
       <c r="B16" t="s">
         <v>14</v>
       </c>
@@ -797,7 +735,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" t="s">
         <v>15</v>
       </c>
@@ -805,7 +743,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" t="s">
         <v>16</v>
       </c>
@@ -813,7 +751,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3">
       <c r="B19" t="s">
         <v>17</v>
       </c>
@@ -821,7 +759,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3">
       <c r="B20" t="s">
         <v>18</v>
       </c>
@@ -829,7 +767,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3">
       <c r="B21" t="s">
         <v>19</v>
       </c>
@@ -837,7 +775,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3">
       <c r="B22" t="s">
         <v>20</v>
       </c>
@@ -845,7 +783,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3">
       <c r="B23" t="s">
         <v>21</v>
       </c>
@@ -853,7 +791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3">
       <c r="B24" t="s">
         <v>22</v>
       </c>
@@ -861,7 +799,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3">
       <c r="B25" t="s">
         <v>23</v>
       </c>
@@ -869,7 +807,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3">
       <c r="B26" t="s">
         <v>24</v>
       </c>
@@ -877,7 +815,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3">
       <c r="B27" t="s">
         <v>25</v>
       </c>
@@ -885,7 +823,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3">
       <c r="B28" t="s">
         <v>26</v>
       </c>
@@ -893,7 +831,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3">
       <c r="B29" t="s">
         <v>27</v>
       </c>
@@ -901,7 +839,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3">
       <c r="B30" t="s">
         <v>28</v>
       </c>
@@ -909,7 +847,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3">
       <c r="B31" t="s">
         <v>29</v>
       </c>
@@ -917,7 +855,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3">
       <c r="B32" t="s">
         <v>30</v>
       </c>
@@ -925,7 +863,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3">
       <c r="B33" t="s">
         <v>31</v>
       </c>
@@ -933,7 +871,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3">
       <c r="B34" t="s">
         <v>32</v>
       </c>
@@ -941,7 +879,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3">
       <c r="B35" t="s">
         <v>33</v>
       </c>
@@ -949,7 +887,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3">
       <c r="B36" t="s">
         <v>34</v>
       </c>
@@ -957,7 +895,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3">
       <c r="B37" t="s">
         <v>35</v>
       </c>
@@ -965,7 +903,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3">
       <c r="B38" t="s">
         <v>36</v>
       </c>
@@ -973,7 +911,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3">
       <c r="B39" t="s">
         <v>37</v>
       </c>
@@ -981,7 +919,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -989,7 +927,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3">
       <c r="B41" t="s">
         <v>39</v>
       </c>
@@ -997,7 +935,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3">
       <c r="B42" t="s">
         <v>40</v>
       </c>
@@ -1005,7 +943,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3">
       <c r="B43" t="s">
         <v>41</v>
       </c>
@@ -1014,8 +952,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>